<commit_message>
reorganização dos dados na pasta etc.
</commit_message>
<xml_diff>
--- a/dados/series_economicas.xlsx
+++ b/dados/series_economicas.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="454">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -34,19 +34,10 @@
     <t xml:space="preserve">selic</t>
   </si>
   <si>
-    <t xml:space="preserve">inflacao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compuls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inad</t>
-  </si>
-  <si>
     <t xml:space="preserve">pib_mensal</t>
   </si>
   <si>
-    <t xml:space="preserve">prod_ind</t>
+    <t xml:space="preserve">inad_ipea</t>
   </si>
   <si>
     <t xml:space="preserve">igp_di</t>
@@ -61,18 +52,12 @@
     <t xml:space="preserve">11.62</t>
   </si>
   <si>
-    <t xml:space="preserve">0.79</t>
+    <t xml:space="preserve">348082.9</t>
   </si>
   <si>
     <t xml:space="preserve">4.41</t>
   </si>
   <si>
-    <t xml:space="preserve">348082.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.666032350142709</t>
-  </si>
-  <si>
     <t xml:space="preserve">7.57210567420323</t>
   </si>
   <si>
@@ -85,15 +70,9 @@
     <t xml:space="preserve">11.74</t>
   </si>
   <si>
-    <t xml:space="preserve">0.77</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.55</t>
   </si>
   <si>
-    <t xml:space="preserve">-1.81268882175226</t>
-  </si>
-  <si>
     <t xml:space="preserve">6.11197908235774</t>
   </si>
   <si>
@@ -106,18 +85,12 @@
     <t xml:space="preserve">11.92</t>
   </si>
   <si>
-    <t xml:space="preserve">0.47</t>
+    <t xml:space="preserve">366411.2</t>
   </si>
   <si>
     <t xml:space="preserve">4.72</t>
   </si>
   <si>
-    <t xml:space="preserve">366411.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.68456375838926</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.0814202983003831</t>
   </si>
   <si>
@@ -130,18 +103,12 @@
     <t xml:space="preserve">12.1</t>
   </si>
   <si>
-    <t xml:space="preserve">0.15</t>
+    <t xml:space="preserve">371046.4</t>
   </si>
   <si>
     <t xml:space="preserve">4.71</t>
   </si>
   <si>
-    <t xml:space="preserve">371046.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.292682926829269</t>
-  </si>
-  <si>
     <t xml:space="preserve">-1.56385958182769</t>
   </si>
   <si>
@@ -154,18 +121,12 @@
     <t xml:space="preserve">12.25</t>
   </si>
   <si>
-    <t xml:space="preserve">0.16</t>
+    <t xml:space="preserve">373333.7</t>
   </si>
   <si>
     <t xml:space="preserve">4.89</t>
   </si>
   <si>
-    <t xml:space="preserve">373333.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.748362956033688</t>
-  </si>
-  <si>
     <t xml:space="preserve">-0.60816911972531</t>
   </si>
   <si>
@@ -178,15 +139,9 @@
     <t xml:space="preserve">12.42</t>
   </si>
   <si>
-    <t xml:space="preserve">0.37</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.96</t>
   </si>
   <si>
-    <t xml:space="preserve">2.49768732654949</t>
-  </si>
-  <si>
     <t xml:space="preserve">7.60953523148764</t>
   </si>
   <si>
@@ -199,18 +154,12 @@
     <t xml:space="preserve">11.91</t>
   </si>
   <si>
-    <t xml:space="preserve">0.53</t>
+    <t xml:space="preserve">361994.5</t>
   </si>
   <si>
     <t xml:space="preserve">4.97</t>
   </si>
   <si>
-    <t xml:space="preserve">361994.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.945179584120981</t>
-  </si>
-  <si>
     <t xml:space="preserve">9.41216022218181</t>
   </si>
   <si>
@@ -223,18 +172,12 @@
     <t xml:space="preserve">11.7</t>
   </si>
   <si>
-    <t xml:space="preserve">0.43</t>
+    <t xml:space="preserve">378842.6</t>
   </si>
   <si>
     <t xml:space="preserve">5.12</t>
   </si>
   <si>
-    <t xml:space="preserve">378842.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.29990714948933</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.87981624223151</t>
   </si>
   <si>
@@ -247,18 +190,12 @@
     <t xml:space="preserve">11.4</t>
   </si>
   <si>
-    <t xml:space="preserve">0.52</t>
+    <t xml:space="preserve">389949.4</t>
   </si>
   <si>
     <t xml:space="preserve">5.16</t>
   </si>
   <si>
-    <t xml:space="preserve">389949.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.43445692883895</t>
-  </si>
-  <si>
     <t xml:space="preserve">5.24398053472293</t>
   </si>
   <si>
@@ -271,18 +208,12 @@
     <t xml:space="preserve">10.9</t>
   </si>
   <si>
-    <t xml:space="preserve">0.5</t>
+    <t xml:space="preserve">392012.5</t>
   </si>
   <si>
     <t xml:space="preserve">5.14</t>
   </si>
   <si>
-    <t xml:space="preserve">392012.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.931677018633537</t>
-  </si>
-  <si>
     <t xml:space="preserve">-1.90033772574818</t>
   </si>
   <si>
@@ -295,15 +226,9 @@
     <t xml:space="preserve">10.7</t>
   </si>
   <si>
-    <t xml:space="preserve">0.56</t>
-  </si>
-  <si>
     <t xml:space="preserve">5.33</t>
   </si>
   <si>
-    <t xml:space="preserve">-4.82832618025751</t>
-  </si>
-  <si>
     <t xml:space="preserve">3.64998814238131</t>
   </si>
   <si>
@@ -316,18 +241,12 @@
     <t xml:space="preserve">10.4</t>
   </si>
   <si>
-    <t xml:space="preserve">0.45</t>
+    <t xml:space="preserve">367852.6</t>
   </si>
   <si>
     <t xml:space="preserve">5.42</t>
   </si>
   <si>
-    <t xml:space="preserve">367852.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-5.8700209643606</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.848717847003178</t>
   </si>
   <si>
@@ -340,15 +259,9 @@
     <t xml:space="preserve">9.82</t>
   </si>
   <si>
-    <t xml:space="preserve">0.21</t>
-  </si>
-  <si>
     <t xml:space="preserve">5.32</t>
   </si>
   <si>
-    <t xml:space="preserve">-4.50191570881227</t>
-  </si>
-  <si>
     <t xml:space="preserve">6.89014233218959</t>
   </si>
   <si>
@@ -358,18 +271,12 @@
     <t xml:space="preserve">9.35</t>
   </si>
   <si>
-    <t xml:space="preserve">0.64</t>
+    <t xml:space="preserve">382581.2</t>
   </si>
   <si>
     <t xml:space="preserve">5.41</t>
   </si>
   <si>
-    <t xml:space="preserve">382581.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4.82051282051282</t>
-  </si>
-  <si>
     <t xml:space="preserve">12.8932289861097</t>
   </si>
   <si>
@@ -382,18 +289,12 @@
     <t xml:space="preserve">8.87</t>
   </si>
   <si>
-    <t xml:space="preserve">0.36</t>
+    <t xml:space="preserve">401072.7</t>
   </si>
   <si>
     <t xml:space="preserve">5.49</t>
   </si>
   <si>
-    <t xml:space="preserve">401072.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4.29505135387488</t>
-  </si>
-  <si>
     <t xml:space="preserve">11.5292382785686</t>
   </si>
   <si>
@@ -406,18 +307,12 @@
     <t xml:space="preserve">8.39</t>
   </si>
   <si>
-    <t xml:space="preserve">0.08</t>
+    <t xml:space="preserve">399470.5</t>
   </si>
   <si>
     <t xml:space="preserve">5.4</t>
   </si>
   <si>
-    <t xml:space="preserve">399470.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4.37743190661478</t>
-  </si>
-  <si>
     <t xml:space="preserve">8.56582219363646</t>
   </si>
   <si>
@@ -430,15 +325,12 @@
     <t xml:space="preserve">8.07</t>
   </si>
   <si>
+    <t xml:space="preserve">415385.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.43</t>
   </si>
   <si>
-    <t xml:space="preserve">415385.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.50801131008482</t>
-  </si>
-  <si>
     <t xml:space="preserve">19.7827930649685</t>
   </si>
   <si>
@@ -451,18 +343,12 @@
     <t xml:space="preserve">7.85</t>
   </si>
   <si>
-    <t xml:space="preserve">0.41</t>
+    <t xml:space="preserve">420727.9</t>
   </si>
   <si>
     <t xml:space="preserve">5.5</t>
   </si>
   <si>
-    <t xml:space="preserve">420727.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.631768953068601</t>
-  </si>
-  <si>
     <t xml:space="preserve">16.6604878420034</t>
   </si>
   <si>
@@ -475,18 +361,12 @@
     <t xml:space="preserve">7.39</t>
   </si>
   <si>
-    <t xml:space="preserve">0.57</t>
+    <t xml:space="preserve">394335.9</t>
   </si>
   <si>
     <t xml:space="preserve">5.45</t>
   </si>
   <si>
-    <t xml:space="preserve">394335.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.33587786259541</t>
-  </si>
-  <si>
     <t xml:space="preserve">11.0881261335594</t>
   </si>
   <si>
@@ -499,18 +379,12 @@
     <t xml:space="preserve">7.23</t>
   </si>
   <si>
-    <t xml:space="preserve">0.59</t>
+    <t xml:space="preserve">423408.3</t>
   </si>
   <si>
     <t xml:space="preserve">5.47</t>
   </si>
   <si>
-    <t xml:space="preserve">423408.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.17403574788335</t>
-  </si>
-  <si>
     <t xml:space="preserve">-3.71290282440302</t>
   </si>
   <si>
@@ -523,18 +397,12 @@
     <t xml:space="preserve">7.14</t>
   </si>
   <si>
-    <t xml:space="preserve">0.6</t>
+    <t xml:space="preserve">424493.8</t>
   </si>
   <si>
     <t xml:space="preserve">5.36</t>
   </si>
   <si>
-    <t xml:space="preserve">424493.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.575815738963525</t>
-  </si>
-  <si>
     <t xml:space="preserve">3.04939230952752</t>
   </si>
   <si>
@@ -547,15 +415,12 @@
     <t xml:space="preserve">7.16</t>
   </si>
   <si>
+    <t xml:space="preserve">423811.8</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.28</t>
   </si>
   <si>
-    <t xml:space="preserve">423811.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3.65726227795193</t>
-  </si>
-  <si>
     <t xml:space="preserve">8.19862317455575</t>
   </si>
   <si>
@@ -568,18 +433,12 @@
     <t xml:space="preserve">7.11</t>
   </si>
   <si>
-    <t xml:space="preserve">0.86</t>
+    <t xml:space="preserve">414583.9</t>
   </si>
   <si>
     <t xml:space="preserve">5.29</t>
   </si>
   <si>
-    <t xml:space="preserve">414583.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.53889515219841</t>
-  </si>
-  <si>
     <t xml:space="preserve">3.75158328365517</t>
   </si>
   <si>
@@ -592,15 +451,12 @@
     <t xml:space="preserve">7.12</t>
   </si>
   <si>
+    <t xml:space="preserve">399106.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.24</t>
   </si>
   <si>
-    <t xml:space="preserve">399106.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.89309576837416</t>
-  </si>
-  <si>
     <t xml:space="preserve">2.40796562667607</t>
   </si>
   <si>
@@ -616,9 +472,6 @@
     <t xml:space="preserve">427931.4</t>
   </si>
   <si>
-    <t xml:space="preserve">-2.00601805416248</t>
-  </si>
-  <si>
     <t xml:space="preserve">3.72254605164082</t>
   </si>
   <si>
@@ -631,12 +484,6 @@
     <t xml:space="preserve">7.26</t>
   </si>
   <si>
-    <t xml:space="preserve">0.55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.69827586206897</t>
-  </si>
-  <si>
     <t xml:space="preserve">-0.679030485378707</t>
   </si>
   <si>
@@ -649,15 +496,12 @@
     <t xml:space="preserve">7.42</t>
   </si>
   <si>
+    <t xml:space="preserve">439658.6</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.15</t>
   </si>
   <si>
-    <t xml:space="preserve">439658.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.4390243902439</t>
-  </si>
-  <si>
     <t xml:space="preserve">3.92135465233612</t>
   </si>
   <si>
@@ -670,18 +514,12 @@
     <t xml:space="preserve">7.9</t>
   </si>
   <si>
-    <t xml:space="preserve">0.26</t>
+    <t xml:space="preserve">443477.5</t>
   </si>
   <si>
     <t xml:space="preserve">4.87</t>
   </si>
   <si>
-    <t xml:space="preserve">443477.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.4587995930824</t>
-  </si>
-  <si>
     <t xml:space="preserve">9.55403228378113</t>
   </si>
   <si>
@@ -694,15 +532,9 @@
     <t xml:space="preserve">8.23</t>
   </si>
   <si>
-    <t xml:space="preserve">0.03</t>
-  </si>
-  <si>
     <t xml:space="preserve">459578.2</t>
   </si>
   <si>
-    <t xml:space="preserve">3.34928229665072</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.68672726523422</t>
   </si>
   <si>
@@ -715,18 +547,12 @@
     <t xml:space="preserve">8.45</t>
   </si>
   <si>
-    <t xml:space="preserve">0.24</t>
+    <t xml:space="preserve">454222.5</t>
   </si>
   <si>
     <t xml:space="preserve">4.77</t>
   </si>
   <si>
-    <t xml:space="preserve">454222.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.448430493273544</t>
-  </si>
-  <si>
     <t xml:space="preserve">5.69565831887349</t>
   </si>
   <si>
@@ -739,18 +565,12 @@
     <t xml:space="preserve">8.9</t>
   </si>
   <si>
-    <t xml:space="preserve">0.35</t>
+    <t xml:space="preserve">440331.5</t>
   </si>
   <si>
     <t xml:space="preserve">4.73</t>
   </si>
   <si>
-    <t xml:space="preserve">440331.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.77176015473888</t>
-  </si>
-  <si>
     <t xml:space="preserve">17.567149787518</t>
   </si>
   <si>
@@ -763,15 +583,12 @@
     <t xml:space="preserve">9.25</t>
   </si>
   <si>
+    <t xml:space="preserve">468524.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">4.63</t>
   </si>
   <si>
-    <t xml:space="preserve">468524.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.715563506261185</t>
-  </si>
-  <si>
     <t xml:space="preserve">7.78585117188852</t>
   </si>
   <si>
@@ -784,18 +601,12 @@
     <t xml:space="preserve">9.45</t>
   </si>
   <si>
-    <t xml:space="preserve">0.54</t>
+    <t xml:space="preserve">468299.2</t>
   </si>
   <si>
     <t xml:space="preserve">4.5</t>
   </si>
   <si>
-    <t xml:space="preserve">468299.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.24045801526718</t>
-  </si>
-  <si>
     <t xml:space="preserve">3.37293414150366</t>
   </si>
   <si>
@@ -808,18 +619,12 @@
     <t xml:space="preserve">9.9</t>
   </si>
   <si>
-    <t xml:space="preserve">0.92</t>
+    <t xml:space="preserve">476455.4</t>
   </si>
   <si>
     <t xml:space="preserve">4.4</t>
   </si>
   <si>
-    <t xml:space="preserve">476455.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.27765726681128</t>
-  </si>
-  <si>
     <t xml:space="preserve">8.5887776352477</t>
   </si>
   <si>
@@ -835,9 +640,6 @@
     <t xml:space="preserve">460551.7</t>
   </si>
   <si>
-    <t xml:space="preserve">-2.01058201058202</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.94663718389323</t>
   </si>
   <si>
@@ -850,18 +652,12 @@
     <t xml:space="preserve">10.43</t>
   </si>
   <si>
-    <t xml:space="preserve">0.69</t>
+    <t xml:space="preserve">456107.7</t>
   </si>
   <si>
     <t xml:space="preserve">4.38</t>
   </si>
   <si>
-    <t xml:space="preserve">456107.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.76730987514189</t>
-  </si>
-  <si>
     <t xml:space="preserve">10.6259842911134</t>
   </si>
   <si>
@@ -874,15 +670,12 @@
     <t xml:space="preserve">10.65</t>
   </si>
   <si>
+    <t xml:space="preserve">469282.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">4.39</t>
   </si>
   <si>
-    <t xml:space="preserve">469282.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.409416581371547</t>
-  </si>
-  <si>
     <t xml:space="preserve">19.3397505723004</t>
   </si>
   <si>
@@ -895,18 +688,12 @@
     <t xml:space="preserve">10.87</t>
   </si>
   <si>
-    <t xml:space="preserve">0.67</t>
+    <t xml:space="preserve">476294.1</t>
   </si>
   <si>
     <t xml:space="preserve">4.43</t>
   </si>
   <si>
-    <t xml:space="preserve">476294.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-5.69744597249509</t>
-  </si>
-  <si>
     <t xml:space="preserve">5.54820292887235</t>
   </si>
   <si>
@@ -916,18 +703,12 @@
     <t xml:space="preserve">24.61</t>
   </si>
   <si>
-    <t xml:space="preserve">0.46</t>
+    <t xml:space="preserve">480663.9</t>
   </si>
   <si>
     <t xml:space="preserve">4.58</t>
   </si>
   <si>
-    <t xml:space="preserve">480663.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3.14285714285714</t>
-  </si>
-  <si>
     <t xml:space="preserve">-5.32320823877979</t>
   </si>
   <si>
@@ -937,18 +718,12 @@
     <t xml:space="preserve">25.09</t>
   </si>
   <si>
-    <t xml:space="preserve">0.4</t>
+    <t xml:space="preserve">465329.8</t>
   </si>
   <si>
     <t xml:space="preserve">4.46</t>
   </si>
   <si>
-    <t xml:space="preserve">465329.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-6.68633235004916</t>
-  </si>
-  <si>
     <t xml:space="preserve">-7.34529640129208</t>
   </si>
   <si>
@@ -958,36 +733,24 @@
     <t xml:space="preserve">25.51</t>
   </si>
   <si>
-    <t xml:space="preserve">0.01</t>
+    <t xml:space="preserve">490265.9</t>
   </si>
   <si>
     <t xml:space="preserve">4.56</t>
   </si>
   <si>
-    <t xml:space="preserve">490265.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3.33333333333333</t>
-  </si>
-  <si>
     <t xml:space="preserve">-6.40799161672404</t>
   </si>
   <si>
     <t xml:space="preserve">2014-08-01</t>
   </si>
   <si>
-    <t xml:space="preserve">0.25</t>
+    <t xml:space="preserve">485883.3</t>
   </si>
   <si>
     <t xml:space="preserve">4.6</t>
   </si>
   <si>
-    <t xml:space="preserve">485883.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-5.08928571428572</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.759292181455451</t>
   </si>
   <si>
@@ -1000,9 +763,6 @@
     <t xml:space="preserve">485984.5</t>
   </si>
   <si>
-    <t xml:space="preserve">-1.58434296365331</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.220405825717207</t>
   </si>
   <si>
@@ -1015,18 +775,12 @@
     <t xml:space="preserve">10.92</t>
   </si>
   <si>
-    <t xml:space="preserve">0.42</t>
+    <t xml:space="preserve">502782.8</t>
   </si>
   <si>
     <t xml:space="preserve">4.61</t>
   </si>
   <si>
-    <t xml:space="preserve">502782.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.93072824156305</t>
-  </si>
-  <si>
     <t xml:space="preserve">7.36194911455827</t>
   </si>
   <si>
@@ -1039,18 +793,12 @@
     <t xml:space="preserve">11.15</t>
   </si>
   <si>
-    <t xml:space="preserve">0.51</t>
+    <t xml:space="preserve">498049.1</t>
   </si>
   <si>
     <t xml:space="preserve">4.45</t>
   </si>
   <si>
-    <t xml:space="preserve">498049.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-5.937794533459</t>
-  </si>
-  <si>
     <t xml:space="preserve">14.5673647683823</t>
   </si>
   <si>
@@ -1063,18 +811,12 @@
     <t xml:space="preserve">11.58</t>
   </si>
   <si>
-    <t xml:space="preserve">0.78</t>
+    <t xml:space="preserve">507757.9</t>
   </si>
   <si>
     <t xml:space="preserve">4.31</t>
   </si>
   <si>
-    <t xml:space="preserve">507757.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.66370699223084</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.70814232695997</t>
   </si>
   <si>
@@ -1084,15 +826,9 @@
     <t xml:space="preserve">11.82</t>
   </si>
   <si>
-    <t xml:space="preserve">1.24</t>
-  </si>
-  <si>
     <t xml:space="preserve">481096.4</t>
   </si>
   <si>
-    <t xml:space="preserve">-4.85961123110151</t>
-  </si>
-  <si>
     <t xml:space="preserve">8.3272970665486</t>
   </si>
   <si>
@@ -1105,18 +841,12 @@
     <t xml:space="preserve">12.15</t>
   </si>
   <si>
-    <t xml:space="preserve">1.22</t>
+    <t xml:space="preserve">466996.4</t>
   </si>
   <si>
     <t xml:space="preserve">4.42</t>
   </si>
   <si>
-    <t xml:space="preserve">466996.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-9.31744312026002</t>
-  </si>
-  <si>
     <t xml:space="preserve">6.61147596850074</t>
   </si>
   <si>
@@ -1129,15 +859,9 @@
     <t xml:space="preserve">12.58</t>
   </si>
   <si>
-    <t xml:space="preserve">1.32</t>
-  </si>
-  <si>
     <t xml:space="preserve">508717.2</t>
   </si>
   <si>
-    <t xml:space="preserve">-3.08324768756424</t>
-  </si>
-  <si>
     <t xml:space="preserve">15.5646354375019</t>
   </si>
   <si>
@@ -1150,15 +874,9 @@
     <t xml:space="preserve">12.68</t>
   </si>
   <si>
-    <t xml:space="preserve">0.71</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.57</t>
   </si>
   <si>
-    <t xml:space="preserve">-7.50000000000001</t>
-  </si>
-  <si>
     <t xml:space="preserve">11.5596488779083</t>
   </si>
   <si>
@@ -1171,18 +889,12 @@
     <t xml:space="preserve">13.15</t>
   </si>
   <si>
-    <t xml:space="preserve">0.74</t>
+    <t xml:space="preserve">491236.3</t>
   </si>
   <si>
     <t xml:space="preserve">4.68</t>
   </si>
   <si>
-    <t xml:space="preserve">491247.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-8.45624385447396</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.94454582485504</t>
   </si>
   <si>
@@ -1195,15 +907,12 @@
     <t xml:space="preserve">13.58</t>
   </si>
   <si>
+    <t xml:space="preserve">495279.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">4.59</t>
   </si>
   <si>
-    <t xml:space="preserve">495290.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.52897787144363</t>
-  </si>
-  <si>
     <t xml:space="preserve">8.50423625874528</t>
   </si>
   <si>
@@ -1216,10 +925,7 @@
     <t xml:space="preserve">13.69</t>
   </si>
   <si>
-    <t xml:space="preserve">0.62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-8.52490421455939</t>
+    <t xml:space="preserve">511103.1</t>
   </si>
   <si>
     <t xml:space="preserve">7.21870577577441</t>
@@ -1234,18 +940,12 @@
     <t xml:space="preserve">14.15</t>
   </si>
   <si>
-    <t xml:space="preserve">0.22</t>
+    <t xml:space="preserve">501180.5</t>
   </si>
   <si>
     <t xml:space="preserve">4.91</t>
   </si>
   <si>
-    <t xml:space="preserve">501204.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-8.18438381937911</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.92396556616905</t>
   </si>
   <si>
@@ -1255,15 +955,12 @@
     <t xml:space="preserve">31.49</t>
   </si>
   <si>
+    <t xml:space="preserve">495898.8</t>
+  </si>
+  <si>
     <t xml:space="preserve">4.92</t>
   </si>
   <si>
-    <t xml:space="preserve">495887.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-10.7007575757576</t>
-  </si>
-  <si>
     <t xml:space="preserve">18.4841305849385</t>
   </si>
   <si>
@@ -1273,18 +970,12 @@
     <t xml:space="preserve">32.64</t>
   </si>
   <si>
-    <t xml:space="preserve">0.82</t>
+    <t xml:space="preserve">517844.2</t>
   </si>
   <si>
     <t xml:space="preserve">5.02</t>
   </si>
   <si>
-    <t xml:space="preserve">517856.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-11.0704483074108</t>
-  </si>
-  <si>
     <t xml:space="preserve">23.2641357790079</t>
   </si>
   <si>
@@ -1294,18 +985,12 @@
     <t xml:space="preserve">33.31</t>
   </si>
   <si>
-    <t xml:space="preserve">1.01</t>
+    <t xml:space="preserve">512543.7</t>
   </si>
   <si>
     <t xml:space="preserve">5.22</t>
   </si>
   <si>
-    <t xml:space="preserve">512518.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-12.2244488977956</t>
-  </si>
-  <si>
     <t xml:space="preserve">15.3183013675309</t>
   </si>
   <si>
@@ -1315,13 +1000,7 @@
     <t xml:space="preserve">31.64</t>
   </si>
   <si>
-    <t xml:space="preserve">0.96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">520367.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-11.9726339794755</t>
+    <t xml:space="preserve">520355.2</t>
   </si>
   <si>
     <t xml:space="preserve">5.43923619519082</t>
@@ -1333,18 +1012,12 @@
     <t xml:space="preserve">34.22</t>
   </si>
   <si>
-    <t xml:space="preserve">1.27</t>
+    <t xml:space="preserve">489413.3</t>
   </si>
   <si>
     <t xml:space="preserve">5.44</t>
   </si>
   <si>
-    <t xml:space="preserve">489413.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-13.3938706015891</t>
-  </si>
-  <si>
     <t xml:space="preserve">20.0168853492424</t>
   </si>
   <si>
@@ -1354,15 +1027,9 @@
     <t xml:space="preserve">35.8</t>
   </si>
   <si>
-    <t xml:space="preserve">0.9</t>
-  </si>
-  <si>
     <t xml:space="preserve">491587.6</t>
   </si>
   <si>
-    <t xml:space="preserve">-9.43847072879331</t>
-  </si>
-  <si>
     <t xml:space="preserve">9.8947942052346</t>
   </si>
   <si>
@@ -1372,15 +1039,12 @@
     <t xml:space="preserve">37.09</t>
   </si>
   <si>
+    <t xml:space="preserve">518347.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.51</t>
   </si>
   <si>
-    <t xml:space="preserve">518347.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-11.2407211028632</t>
-  </si>
-  <si>
     <t xml:space="preserve">5.30239099501644</t>
   </si>
   <si>
@@ -1390,18 +1054,12 @@
     <t xml:space="preserve">38.74</t>
   </si>
   <si>
-    <t xml:space="preserve">0.61</t>
+    <t xml:space="preserve">509687.5</t>
   </si>
   <si>
     <t xml:space="preserve">5.65</t>
   </si>
   <si>
-    <t xml:space="preserve">509687.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-6.53153153153153</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.46149974084822</t>
   </si>
   <si>
@@ -1411,15 +1069,12 @@
     <t xml:space="preserve">39.2</t>
   </si>
   <si>
+    <t xml:space="preserve">513155.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.79</t>
   </si>
   <si>
-    <t xml:space="preserve">513155.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-7.30397422126745</t>
-  </si>
-  <si>
     <t xml:space="preserve">14.459921996055</t>
   </si>
   <si>
@@ -1429,15 +1084,12 @@
     <t xml:space="preserve">39.09</t>
   </si>
   <si>
+    <t xml:space="preserve">535366.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.62</t>
   </si>
   <si>
-    <t xml:space="preserve">535366.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-5.18918918918918</t>
-  </si>
-  <si>
     <t xml:space="preserve">21.4700276265392</t>
   </si>
   <si>
@@ -1447,15 +1099,12 @@
     <t xml:space="preserve">39.9</t>
   </si>
   <si>
+    <t xml:space="preserve">532400.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.7</t>
   </si>
   <si>
-    <t xml:space="preserve">532400.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-6.1780104712042</t>
-  </si>
-  <si>
     <t xml:space="preserve">-4.56174010968963</t>
   </si>
   <si>
@@ -1465,18 +1114,12 @@
     <t xml:space="preserve">40.38</t>
   </si>
   <si>
-    <t xml:space="preserve">0.44</t>
+    <t xml:space="preserve">533434.4</t>
   </si>
   <si>
     <t xml:space="preserve">5.76</t>
   </si>
   <si>
-    <t xml:space="preserve">533434.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4.71311475409836</t>
-  </si>
-  <si>
     <t xml:space="preserve">5.33509782054165</t>
   </si>
   <si>
@@ -1486,15 +1129,12 @@
     <t xml:space="preserve">40.97</t>
   </si>
   <si>
+    <t xml:space="preserve">510941.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.78</t>
   </si>
   <si>
-    <t xml:space="preserve">510941.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3.81760339342523</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.384511023609013</t>
   </si>
   <si>
@@ -1507,10 +1147,7 @@
     <t xml:space="preserve">14.05</t>
   </si>
   <si>
-    <t xml:space="preserve">525380.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-7.20164609053497</t>
+    <t xml:space="preserve">525394.4</t>
   </si>
   <si>
     <t xml:space="preserve">1.5927008740245</t>
@@ -1525,18 +1162,12 @@
     <t xml:space="preserve">13.9</t>
   </si>
   <si>
-    <t xml:space="preserve">0.18</t>
+    <t xml:space="preserve">540879.5</t>
   </si>
   <si>
     <t xml:space="preserve">5.74</t>
   </si>
   <si>
-    <t xml:space="preserve">540865.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.25570776255707</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.646138338215008</t>
   </si>
   <si>
@@ -1549,15 +1180,12 @@
     <t xml:space="preserve">13.65</t>
   </si>
   <si>
-    <t xml:space="preserve">0.3</t>
+    <t xml:space="preserve">566597.7</t>
   </si>
   <si>
     <t xml:space="preserve">5.63</t>
   </si>
   <si>
-    <t xml:space="preserve">566625.4</t>
-  </si>
-  <si>
     <t xml:space="preserve">10.4415626810591</t>
   </si>
   <si>
@@ -1570,15 +1198,12 @@
     <t xml:space="preserve">13.17</t>
   </si>
   <si>
-    <t xml:space="preserve">0.38</t>
+    <t xml:space="preserve">526821.7</t>
   </si>
   <si>
     <t xml:space="preserve">5.67</t>
   </si>
   <si>
-    <t xml:space="preserve">2.09698558322413</t>
-  </si>
-  <si>
     <t xml:space="preserve">5.31267969387728</t>
   </si>
   <si>
@@ -1591,18 +1216,12 @@
     <t xml:space="preserve">12.82</t>
   </si>
   <si>
-    <t xml:space="preserve">0.33</t>
+    <t xml:space="preserve">514116.8</t>
   </si>
   <si>
     <t xml:space="preserve">5.57</t>
   </si>
   <si>
-    <t xml:space="preserve">514103.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.13192612137205</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.75720815196032</t>
   </si>
   <si>
@@ -1612,15 +1231,12 @@
     <t xml:space="preserve">41.81</t>
   </si>
   <si>
+    <t xml:space="preserve">542595.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.72</t>
   </si>
   <si>
-    <t xml:space="preserve">542623.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.0310633213859</t>
-  </si>
-  <si>
     <t xml:space="preserve">-4.4390530419437</t>
   </si>
   <si>
@@ -1633,18 +1249,12 @@
     <t xml:space="preserve">11.59</t>
   </si>
   <si>
-    <t xml:space="preserve">0.14</t>
+    <t xml:space="preserve">523415.3</t>
   </si>
   <si>
     <t xml:space="preserve">5.73</t>
   </si>
   <si>
-    <t xml:space="preserve">523402.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4.45783132530121</t>
-  </si>
-  <si>
     <t xml:space="preserve">-13.9341129724377</t>
   </si>
   <si>
@@ -1654,15 +1264,12 @@
     <t xml:space="preserve">37.36</t>
   </si>
   <si>
-    <t xml:space="preserve">0.31</t>
+    <t xml:space="preserve">547408.5</t>
   </si>
   <si>
     <t xml:space="preserve">5.94</t>
   </si>
   <si>
-    <t xml:space="preserve">4.40324449594438</t>
-  </si>
-  <si>
     <t xml:space="preserve">-5.97837013991186</t>
   </si>
   <si>
@@ -1675,18 +1282,12 @@
     <t xml:space="preserve">10.15</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.23</t>
+    <t xml:space="preserve">555921.3</t>
   </si>
   <si>
     <t xml:space="preserve">5.54</t>
   </si>
   <si>
-    <t xml:space="preserve">555947.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.798175598631712</t>
-  </si>
-  <si>
     <t xml:space="preserve">-10.9403632225159</t>
   </si>
   <si>
@@ -1699,12 +1300,6 @@
     <t xml:space="preserve">10.01</t>
   </si>
   <si>
-    <t xml:space="preserve">556550.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.79017857142858</t>
-  </si>
-  <si>
     <t xml:space="preserve">-3.48607281430331</t>
   </si>
   <si>
@@ -1717,15 +1312,12 @@
     <t xml:space="preserve">9.15</t>
   </si>
   <si>
-    <t xml:space="preserve">0.19</t>
+    <t xml:space="preserve">554736.8</t>
   </si>
   <si>
     <t xml:space="preserve">5.6</t>
   </si>
   <si>
-    <t xml:space="preserve">3.97849462365591</t>
-  </si>
-  <si>
     <t xml:space="preserve">2.90188404354921</t>
   </si>
   <si>
@@ -1738,10 +1330,7 @@
     <t xml:space="preserve">8.35</t>
   </si>
   <si>
-    <t xml:space="preserve">528276.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.53583241455346</t>
+    <t xml:space="preserve">528302.9</t>
   </si>
   <si>
     <t xml:space="preserve">7.6836367729924</t>
@@ -1756,15 +1345,12 @@
     <t xml:space="preserve">8.01</t>
   </si>
   <si>
+    <t xml:space="preserve">549373.8</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.39</t>
   </si>
   <si>
-    <t xml:space="preserve">549374.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.43237250554323</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.17698059031486</t>
   </si>
   <si>
@@ -1777,18 +1363,12 @@
     <t xml:space="preserve">7.4</t>
   </si>
   <si>
-    <t xml:space="preserve">0.28</t>
+    <t xml:space="preserve">565746.9</t>
   </si>
   <si>
     <t xml:space="preserve">5.26</t>
   </si>
   <si>
-    <t xml:space="preserve">565746.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.73988439306359</t>
-  </si>
-  <si>
     <t xml:space="preserve">10.0599531280375</t>
   </si>
   <si>
@@ -1798,10 +1378,7 @@
     <t xml:space="preserve">31.74</t>
   </si>
   <si>
-    <t xml:space="preserve">588865.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.92227979274611</t>
+    <t xml:space="preserve">588865.5</t>
   </si>
   <si>
     <t xml:space="preserve">9.26754863984329</t>
@@ -1905,7 +1482,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1917,13 +1494,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1948,2638 +1522,1891 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1357</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>71575256</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1357</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>64619909</v>
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>349255</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>349255</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1357</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>69425040</v>
+        <v>21</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1361</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>81506620</v>
+        <v>27</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1361</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>70147512</v>
+        <v>33</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1361</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>66752810</v>
+        <v>38</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>377006</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>377006</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1359</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>71815456</v>
+        <v>44</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1359</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>70272118</v>
+        <v>50</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1359</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>61817831</v>
+        <v>56</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>57</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1385</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>79526272</v>
+        <v>62</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>63</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1385</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>89167168</v>
+        <v>67</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>367752</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>68</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>367752</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1385</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>70409247</v>
+        <v>73</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>74</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1385</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>81954870</v>
+        <v>78</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>393868</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>79</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>393868</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1385</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>70080178</v>
+        <v>83</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1385</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>68332378</v>
+        <v>89</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>90</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1405</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>72806508</v>
+        <v>95</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>96</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1405</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>75064184</v>
+        <v>101</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1405</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>73456550</v>
+        <v>107</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>108</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1419</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>68385395</v>
+        <v>113</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>114</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1419</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>158</v>
+        <v>118</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>70229520</v>
+        <v>119</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>163</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>164</v>
+        <v>122</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1419</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>165</v>
+        <v>123</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>166</v>
+        <v>124</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>71222187</v>
+        <v>125</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1465</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>174</v>
+        <v>130</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>76694633</v>
+        <v>131</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>132</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>178</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>179</v>
+        <v>134</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1465</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>181</v>
+        <v>136</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <v>76907060</v>
+        <v>137</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>138</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>186</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>187</v>
+        <v>140</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>1465</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>188</v>
+        <v>141</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>189</v>
+        <v>142</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>68717234</v>
+        <v>143</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>144</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>193</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>194</v>
+        <v>146</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1474</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>195</v>
+        <v>147</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>196</v>
+        <v>148</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>68922878</v>
+        <v>149</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>199</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>200</v>
+        <v>151</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1474</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>201</v>
+        <v>152</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="F27" s="0" t="n">
-        <v>72148462</v>
+        <v>153</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>439450</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="H27" s="0" t="n">
-        <v>439450</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>205</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>206</v>
+        <v>155</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1474</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>207</v>
+        <v>156</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>208</v>
+        <v>157</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <v>61551792</v>
+        <v>158</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>159</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>212</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>213</v>
+        <v>161</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1516</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>214</v>
+        <v>162</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>215</v>
+        <v>163</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="F29" s="0" t="n">
-        <v>75727378</v>
+        <v>164</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>165</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="J29" s="0" t="s">
-        <v>220</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>221</v>
+        <v>167</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1516</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>222</v>
+        <v>168</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>223</v>
+        <v>169</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="F30" s="0" t="n">
-        <v>68670039</v>
+        <v>170</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>165</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="J30" s="0" t="s">
-        <v>227</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>228</v>
+        <v>172</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1516</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>229</v>
+        <v>173</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>230</v>
+        <v>174</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="F31" s="0" t="n">
-        <v>65930852</v>
+        <v>175</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>176</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="J31" s="0" t="s">
-        <v>235</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>236</v>
+        <v>178</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1540</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>237</v>
+        <v>179</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>238</v>
+        <v>180</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <v>80920411</v>
+        <v>181</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>182</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="J32" s="0" t="s">
-        <v>243</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>244</v>
+        <v>184</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1540</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>245</v>
+        <v>185</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>246</v>
+        <v>186</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="F33" s="0" t="n">
-        <v>63304977</v>
+        <v>187</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>188</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="J33" s="0" t="s">
-        <v>250</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>251</v>
+        <v>190</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1540</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>252</v>
+        <v>191</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>253</v>
+        <v>192</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="F34" s="0" t="n">
-        <v>61884038</v>
+        <v>193</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>194</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="J34" s="0" t="s">
-        <v>258</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>259</v>
+        <v>196</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1566</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>260</v>
+        <v>197</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>261</v>
+        <v>198</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="F35" s="0" t="n">
-        <v>76504971</v>
+        <v>199</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>200</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="J35" s="0" t="s">
-        <v>266</v>
+        <v>201</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>267</v>
+        <v>202</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1566</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>268</v>
+        <v>203</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>269</v>
+        <v>204</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="F36" s="0" t="n">
-        <v>67781882</v>
+        <v>205</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>200</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="J36" s="0" t="s">
-        <v>272</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>273</v>
+        <v>207</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1566</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>274</v>
+        <v>208</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>275</v>
+        <v>209</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="F37" s="0" t="n">
-        <v>63030469</v>
+        <v>210</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>211</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="J37" s="0" t="s">
-        <v>280</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>281</v>
+        <v>213</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1579</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>282</v>
+        <v>214</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>283</v>
+        <v>215</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="F38" s="0" t="n">
-        <v>75011630</v>
+        <v>216</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>217</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="I38" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="J38" s="0" t="s">
-        <v>287</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>288</v>
+        <v>219</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1579</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>289</v>
+        <v>220</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>290</v>
+        <v>221</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="F39" s="0" t="n">
-        <v>69018203</v>
+        <v>222</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>223</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="H39" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="I39" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="J39" s="0" t="s">
-        <v>295</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>296</v>
+        <v>225</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1579</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>297</v>
+        <v>226</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="F40" s="0" t="n">
-        <v>62602655</v>
+        <v>227</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>228</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="H40" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="I40" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="J40" s="0" t="s">
-        <v>302</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>303</v>
+        <v>230</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1612</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>304</v>
+        <v>231</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="F41" s="0" t="n">
-        <v>66593691</v>
+        <v>232</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>233</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="H41" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="J41" s="0" t="s">
-        <v>309</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>310</v>
+        <v>235</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1612</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>311</v>
+        <v>236</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="F42" s="0" t="n">
-        <v>67056857</v>
+        <v>237</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>238</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="I42" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="J42" s="0" t="s">
-        <v>316</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>317</v>
+        <v>240</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1612</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>311</v>
+        <v>236</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="F43" s="0" t="n">
-        <v>71383450</v>
+        <v>241</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>242</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="H43" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="J43" s="0" t="s">
-        <v>322</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>323</v>
+        <v>244</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1617</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>324</v>
+        <v>245</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <v>73838715</v>
+        <v>246</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>228</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="H44" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="I44" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="J44" s="0" t="s">
-        <v>327</v>
+        <v>247</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>328</v>
+        <v>248</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1617</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>329</v>
+        <v>249</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>330</v>
+        <v>250</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="F45" s="0" t="n">
-        <v>66321390</v>
+        <v>251</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>252</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>332</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="I45" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="J45" s="0" t="s">
-        <v>335</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>336</v>
+        <v>254</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1617</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>337</v>
+        <v>255</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>338</v>
+        <v>256</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="F46" s="0" t="n">
-        <v>70357116</v>
+        <v>257</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>258</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>340</v>
-      </c>
-      <c r="H46" s="0" t="s">
-        <v>341</v>
-      </c>
-      <c r="I46" s="0" t="s">
-        <v>342</v>
-      </c>
-      <c r="J46" s="0" t="s">
-        <v>343</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>344</v>
+        <v>260</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>1628</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>345</v>
+        <v>261</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>346</v>
+        <v>262</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="F47" s="0" t="n">
-        <v>73897496</v>
+        <v>263</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>264</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="I47" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="J47" s="0" t="s">
-        <v>351</v>
+        <v>265</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>352</v>
+        <v>266</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1628</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>353</v>
+        <v>267</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="F48" s="0" t="n">
-        <v>69053687</v>
+        <v>268</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H48" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="I48" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="J48" s="0" t="s">
-        <v>357</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>358</v>
+        <v>270</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>1628</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>359</v>
+        <v>271</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>360</v>
+        <v>272</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>361</v>
-      </c>
-      <c r="F49" s="0" t="n">
-        <v>69858800</v>
+        <v>273</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>274</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="H49" s="0" t="s">
-        <v>363</v>
-      </c>
-      <c r="I49" s="0" t="s">
-        <v>364</v>
-      </c>
-      <c r="J49" s="0" t="s">
-        <v>365</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>366</v>
+        <v>276</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1624</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>367</v>
+        <v>277</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>368</v>
+        <v>278</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="F50" s="0" t="n">
-        <v>69611820</v>
+        <v>279</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>211</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="H50" s="0" t="s">
-        <v>370</v>
-      </c>
-      <c r="I50" s="0" t="s">
-        <v>371</v>
-      </c>
-      <c r="J50" s="0" t="s">
-        <v>372</v>
+        <v>280</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>373</v>
+        <v>281</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>1624</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>374</v>
+        <v>282</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>375</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>376</v>
-      </c>
-      <c r="F51" s="0" t="n">
-        <v>65474383</v>
+        <v>283</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>493536</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>284</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>377</v>
-      </c>
-      <c r="H51" s="0" t="n">
-        <v>493513</v>
-      </c>
-      <c r="I51" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="J51" s="0" t="s">
-        <v>379</v>
+        <v>285</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>380</v>
+        <v>286</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>1624</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>381</v>
+        <v>287</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>382</v>
+        <v>288</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>383</v>
-      </c>
-      <c r="F52" s="0" t="n">
-        <v>72549365</v>
+        <v>289</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>290</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>384</v>
-      </c>
-      <c r="H52" s="0" t="s">
-        <v>385</v>
-      </c>
-      <c r="I52" s="0" t="s">
-        <v>386</v>
-      </c>
-      <c r="J52" s="0" t="s">
-        <v>387</v>
+        <v>291</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>388</v>
+        <v>292</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>1647</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>389</v>
+        <v>293</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>390</v>
+        <v>294</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" s="0" t="n">
-        <v>63989524</v>
+        <v>295</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>296</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="H53" s="0" t="s">
-        <v>392</v>
-      </c>
-      <c r="I53" s="0" t="s">
-        <v>393</v>
-      </c>
-      <c r="J53" s="0" t="s">
-        <v>394</v>
+        <v>297</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>395</v>
+        <v>298</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1647</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>396</v>
+        <v>299</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>397</v>
+        <v>300</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="F54" s="0" t="n">
-        <v>56126083</v>
+        <v>301</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>176</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="H54" s="0" t="n">
-        <v>511091</v>
-      </c>
-      <c r="I54" s="0" t="s">
-        <v>399</v>
-      </c>
-      <c r="J54" s="0" t="s">
-        <v>400</v>
+        <v>302</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>401</v>
+        <v>303</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>1647</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>402</v>
+        <v>304</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>404</v>
-      </c>
-      <c r="F55" s="0" t="n">
-        <v>63339631</v>
+        <v>306</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>307</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>405</v>
-      </c>
-      <c r="H55" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="I55" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="J55" s="0" t="s">
-        <v>408</v>
+        <v>308</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>409</v>
+        <v>309</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>1589</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>410</v>
+        <v>310</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="F56" s="0" t="n">
-        <v>59054581</v>
+        <v>311</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>312</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>411</v>
-      </c>
-      <c r="H56" s="0" t="s">
-        <v>412</v>
-      </c>
-      <c r="I56" s="0" t="s">
-        <v>413</v>
-      </c>
-      <c r="J56" s="0" t="s">
-        <v>414</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>415</v>
+        <v>314</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>1589</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>416</v>
+        <v>315</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>417</v>
-      </c>
-      <c r="F57" s="0" t="n">
-        <v>63492822</v>
+        <v>316</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>317</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>418</v>
-      </c>
-      <c r="H57" s="0" t="s">
-        <v>419</v>
-      </c>
-      <c r="I57" s="0" t="s">
-        <v>420</v>
-      </c>
-      <c r="J57" s="0" t="s">
-        <v>421</v>
+        <v>318</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>422</v>
+        <v>319</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>1589</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>423</v>
+        <v>320</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>424</v>
-      </c>
-      <c r="F58" s="0" t="n">
-        <v>63975642</v>
+        <v>321</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>322</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>425</v>
-      </c>
-      <c r="H58" s="0" t="s">
-        <v>426</v>
-      </c>
-      <c r="I58" s="0" t="s">
-        <v>427</v>
-      </c>
-      <c r="J58" s="0" t="s">
-        <v>428</v>
+        <v>323</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>429</v>
+        <v>324</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>1624</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>430</v>
+        <v>325</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="F59" s="0" t="n">
-        <v>58997463</v>
+        <v>326</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>132</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="H59" s="0" t="s">
-        <v>432</v>
-      </c>
-      <c r="I59" s="0" t="s">
-        <v>433</v>
-      </c>
-      <c r="J59" s="0" t="s">
-        <v>434</v>
+        <v>327</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>435</v>
+        <v>328</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>1624</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>436</v>
+        <v>329</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>437</v>
-      </c>
-      <c r="F60" s="0" t="n">
-        <v>61235516</v>
+        <v>330</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>331</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>438</v>
-      </c>
-      <c r="H60" s="0" t="s">
-        <v>439</v>
-      </c>
-      <c r="I60" s="0" t="s">
-        <v>440</v>
-      </c>
-      <c r="J60" s="0" t="s">
-        <v>441</v>
+        <v>332</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>442</v>
+        <v>333</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>1624</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>443</v>
+        <v>334</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>444</v>
-      </c>
-      <c r="F61" s="0" t="n">
-        <v>75443124</v>
+        <v>335</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="H61" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="I61" s="0" t="s">
-        <v>446</v>
-      </c>
-      <c r="J61" s="0" t="s">
-        <v>447</v>
+        <v>336</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>448</v>
+        <v>337</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>1648</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>449</v>
+        <v>338</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F62" s="0" t="n">
-        <v>65006689</v>
+        <v>339</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>340</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>450</v>
-      </c>
-      <c r="H62" s="0" t="s">
-        <v>451</v>
-      </c>
-      <c r="I62" s="0" t="s">
-        <v>452</v>
-      </c>
-      <c r="J62" s="0" t="s">
-        <v>453</v>
+        <v>341</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>454</v>
+        <v>342</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>1648</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>455</v>
+        <v>343</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>456</v>
-      </c>
-      <c r="F63" s="0" t="n">
-        <v>66297304</v>
+        <v>344</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>345</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>457</v>
-      </c>
-      <c r="H63" s="0" t="s">
-        <v>458</v>
-      </c>
-      <c r="I63" s="0" t="s">
-        <v>459</v>
-      </c>
-      <c r="J63" s="0" t="s">
-        <v>460</v>
+        <v>346</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>461</v>
+        <v>347</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>1648</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>462</v>
+        <v>348</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="F64" s="0" t="n">
-        <v>63559081</v>
+        <v>349</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>350</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>463</v>
-      </c>
-      <c r="H64" s="0" t="s">
-        <v>464</v>
-      </c>
-      <c r="I64" s="0" t="s">
-        <v>465</v>
-      </c>
-      <c r="J64" s="0" t="s">
-        <v>466</v>
+        <v>351</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>467</v>
+        <v>352</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>1742</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>468</v>
+        <v>353</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="F65" s="0" t="n">
-        <v>58697103</v>
+        <v>354</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>355</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>469</v>
-      </c>
-      <c r="H65" s="0" t="s">
-        <v>470</v>
-      </c>
-      <c r="I65" s="0" t="s">
-        <v>471</v>
-      </c>
-      <c r="J65" s="0" t="s">
-        <v>472</v>
+        <v>356</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>473</v>
+        <v>357</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>1742</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>474</v>
+        <v>358</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F66" s="0" t="n">
-        <v>64730531</v>
+        <v>359</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>360</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>475</v>
-      </c>
-      <c r="H66" s="0" t="s">
-        <v>476</v>
-      </c>
-      <c r="I66" s="0" t="s">
-        <v>477</v>
-      </c>
-      <c r="J66" s="0" t="s">
-        <v>478</v>
+        <v>361</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>479</v>
+        <v>362</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>1742</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>480</v>
+        <v>363</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="F67" s="0" t="n">
-        <v>59711693</v>
+        <v>364</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>365</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>482</v>
-      </c>
-      <c r="H67" s="0" t="s">
-        <v>483</v>
-      </c>
-      <c r="I67" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="J67" s="0" t="s">
-        <v>485</v>
+        <v>366</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>486</v>
+        <v>367</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>1715</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>487</v>
+        <v>368</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="F68" s="0" t="n">
-        <v>64370771</v>
+        <v>369</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>370</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>488</v>
-      </c>
-      <c r="H68" s="0" t="s">
-        <v>489</v>
-      </c>
-      <c r="I68" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="J68" s="0" t="s">
-        <v>491</v>
+        <v>371</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>492</v>
+        <v>372</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>1715</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>493</v>
+        <v>373</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>494</v>
+        <v>374</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="F69" s="0" t="n">
-        <v>66686598</v>
+        <v>375</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>350</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>463</v>
-      </c>
-      <c r="H69" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="I69" s="0" t="s">
-        <v>496</v>
-      </c>
-      <c r="J69" s="0" t="s">
-        <v>497</v>
+        <v>376</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>498</v>
+        <v>377</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>1715</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>499</v>
+        <v>378</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>500</v>
+        <v>379</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>501</v>
-      </c>
-      <c r="F70" s="0" t="n">
-        <v>62181615</v>
+        <v>380</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>381</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>502</v>
-      </c>
-      <c r="H70" s="0" t="s">
-        <v>503</v>
-      </c>
-      <c r="I70" s="0" t="s">
-        <v>504</v>
-      </c>
-      <c r="J70" s="0" t="s">
-        <v>505</v>
+        <v>382</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>506</v>
+        <v>383</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>1742</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>507</v>
+        <v>384</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>508</v>
+        <v>385</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>509</v>
-      </c>
-      <c r="F71" s="0" t="n">
-        <v>67584004</v>
+        <v>386</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>387</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>510</v>
-      </c>
-      <c r="H71" s="0" t="s">
-        <v>511</v>
-      </c>
-      <c r="I71" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J71" s="0" t="s">
-        <v>512</v>
+        <v>388</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>513</v>
+        <v>389</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>1742</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>514</v>
+        <v>390</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>515</v>
+        <v>391</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>516</v>
-      </c>
-      <c r="F72" s="0" t="n">
-        <v>78641242</v>
+        <v>392</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>393</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>517</v>
-      </c>
-      <c r="H72" s="0" t="n">
-        <v>526807</v>
-      </c>
-      <c r="I72" s="0" t="s">
-        <v>518</v>
-      </c>
-      <c r="J72" s="0" t="s">
-        <v>519</v>
+        <v>394</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>520</v>
+        <v>395</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>1742</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>521</v>
+        <v>396</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>522</v>
+        <v>397</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>523</v>
-      </c>
-      <c r="F73" s="0" t="n">
-        <v>76462099</v>
+        <v>398</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>399</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="H73" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="I73" s="0" t="s">
-        <v>526</v>
-      </c>
-      <c r="J73" s="0" t="s">
-        <v>527</v>
+        <v>400</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>528</v>
+        <v>401</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>1741</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>529</v>
+        <v>402</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>360</v>
+        <v>272</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="F74" s="0" t="n">
-        <v>62464721</v>
+        <v>403</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>404</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>530</v>
-      </c>
-      <c r="H74" s="0" t="s">
-        <v>531</v>
-      </c>
-      <c r="I74" s="0" t="s">
-        <v>532</v>
-      </c>
-      <c r="J74" s="0" t="s">
-        <v>533</v>
+        <v>405</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>534</v>
+        <v>406</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>1741</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>535</v>
+        <v>407</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>536</v>
+        <v>408</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>537</v>
-      </c>
-      <c r="F75" s="0" t="n">
-        <v>77230243</v>
+        <v>409</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>410</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>538</v>
-      </c>
-      <c r="H75" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="I75" s="0" t="s">
-        <v>540</v>
-      </c>
-      <c r="J75" s="0" t="s">
-        <v>541</v>
+        <v>411</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>542</v>
+        <v>412</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>1741</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>543</v>
+        <v>413</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>338</v>
+        <v>256</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>544</v>
-      </c>
-      <c r="F76" s="0" t="n">
-        <v>55125117</v>
+        <v>414</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>415</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>545</v>
-      </c>
-      <c r="H76" s="0" t="n">
-        <v>547395</v>
-      </c>
-      <c r="I76" s="0" t="s">
-        <v>546</v>
-      </c>
-      <c r="J76" s="0" t="s">
-        <v>547</v>
+        <v>416</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>548</v>
+        <v>417</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>1741</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>549</v>
+        <v>418</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>550</v>
+        <v>419</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>551</v>
-      </c>
-      <c r="F77" s="0" t="n">
-        <v>74108897</v>
+        <v>420</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>421</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>552</v>
-      </c>
-      <c r="H77" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="I77" s="0" t="s">
-        <v>554</v>
-      </c>
-      <c r="J77" s="0" t="s">
-        <v>555</v>
+        <v>422</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>556</v>
+        <v>423</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1741</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>557</v>
+        <v>424</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>558</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="F78" s="0" t="n">
-        <v>68112449</v>
+        <v>425</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>556538</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>355</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>469</v>
-      </c>
-      <c r="H78" s="0" t="s">
-        <v>559</v>
-      </c>
-      <c r="I78" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="J78" s="0" t="s">
-        <v>561</v>
+        <v>426</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>562</v>
+        <v>427</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>1741</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>563</v>
+        <v>428</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>564</v>
+        <v>429</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>565</v>
-      </c>
-      <c r="F79" s="0" t="n">
-        <v>66014596</v>
+        <v>430</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>431</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H79" s="0" t="n">
-        <v>554750</v>
-      </c>
-      <c r="I79" s="0" t="s">
-        <v>567</v>
-      </c>
-      <c r="J79" s="0" t="s">
-        <v>568</v>
+        <v>432</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>569</v>
+        <v>433</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>1751</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>570</v>
+        <v>434</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>571</v>
+        <v>435</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F80" s="0" t="n">
-        <v>72349860</v>
+        <v>436</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="H80" s="0" t="s">
-        <v>572</v>
-      </c>
-      <c r="I80" s="0" t="s">
-        <v>573</v>
-      </c>
-      <c r="J80" s="0" t="s">
-        <v>574</v>
+        <v>437</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>575</v>
+        <v>438</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>1751</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>576</v>
+        <v>439</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>577</v>
+        <v>440</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="F81" s="0" t="n">
-        <v>63010629</v>
+        <v>441</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>442</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>578</v>
-      </c>
-      <c r="H81" s="0" t="s">
-        <v>579</v>
-      </c>
-      <c r="I81" s="0" t="s">
-        <v>580</v>
-      </c>
-      <c r="J81" s="0" t="s">
-        <v>581</v>
+        <v>443</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>582</v>
+        <v>444</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>1751</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>583</v>
+        <v>445</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>584</v>
+        <v>446</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="F82" s="0" t="n">
-        <v>69406447</v>
+        <v>447</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>448</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>586</v>
-      </c>
-      <c r="H82" s="0" t="s">
-        <v>587</v>
-      </c>
-      <c r="I82" s="0" t="s">
-        <v>588</v>
-      </c>
-      <c r="J82" s="0" t="s">
-        <v>589</v>
+        <v>449</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>590</v>
+        <v>450</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>1741</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>591</v>
+        <v>451</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>7</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="F83" s="0" t="n">
-        <v>74445469</v>
+        <v>452</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>307</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>405</v>
-      </c>
-      <c r="H83" s="0" t="s">
-        <v>592</v>
-      </c>
-      <c r="I83" s="0" t="s">
-        <v>593</v>
-      </c>
-      <c r="J83" s="0" t="s">
-        <v>594</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>